<commit_message>
jz- a shit load of changes
</commit_message>
<xml_diff>
--- a/MIL.RTI.CourseDocumentGenerator/MIL.RTI.CourseDocumentGenerator/Files/13M10/Individual_Student_Progress_Sheet_13M10_Phase1.xlsx
+++ b/MIL.RTI.CourseDocumentGenerator/MIL.RTI.CourseDocumentGenerator/Files/13M10/Individual_Student_Progress_Sheet_13M10_Phase1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\github\CourseDocumentGenerator\MIL.RTI.CourseDocumentGenerator\MIL.RTI.CourseDocumentGenerator\Files\13M10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D54A14-2B03-46D3-B3FD-44EF0DB39CCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A07075-B27C-4597-BE59-8F45128C2367}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>GO</t>
   </si>
@@ -37,23 +37,111 @@
     <t>Individual Student Progress Sheet</t>
   </si>
   <si>
-    <t>Verified BY:________________________________</t>
-  </si>
-  <si>
     <t>2nd Bn, 196TH REGT (RTISD)</t>
   </si>
   <si>
     <t xml:space="preserve">Name:      </t>
   </si>
   <si>
-    <t>13M10 MOSQ Phase 1              TASK NUMBER</t>
+    <t>13M1O MOSQ              TASK NUMBER</t>
+  </si>
+  <si>
+    <t>GS61PR / Position and Roles of an MLRS/HIMARS Crewmembers</t>
+  </si>
+  <si>
+    <t>GS61EM / Operate an Interactive Electronic Technical Manual</t>
+  </si>
+  <si>
+    <t>GS61DB / Perform Gunner’s Duties on an M270A1 MLRS/M142 HIMARS</t>
+  </si>
+  <si>
+    <t>GS61SG / Perform Tactical Communications Using SINCGARS</t>
+  </si>
+  <si>
+    <t>GS6100 / Conduct SINCGARS Examination and Review</t>
+  </si>
+  <si>
+    <t>GS61HR / Operate AN/PRC-150(C) HARRIS Radio</t>
+  </si>
+  <si>
+    <t>GS61A1 / Introduction to the M270A1</t>
+  </si>
+  <si>
+    <t>GS61MT / Perform PMCS on an M993A1 Carrier Vehicle</t>
+  </si>
+  <si>
+    <t>GS6121 / M270A1 MLRS PMCS Performance Examination and Critique</t>
+  </si>
+  <si>
+    <t>GS61DD / Operate an M993A1 Carrier Vehicle during a Fire Mission</t>
+  </si>
+  <si>
+    <t>GS61RL / Perform Driver’s Duties during an M270A1 MLRS Reload</t>
+  </si>
+  <si>
+    <t>GS6120 / M270A1 MLRS Launcher Performance Examination and Critique</t>
+  </si>
+  <si>
+    <t>GS61HM / Perform PMCS on an M985A4 HEMTT and M989A1 HEMAT</t>
+  </si>
+  <si>
+    <t>GS61RS / Perform Ammunition Resupply Procedures with an M985A4 HEMTT</t>
+  </si>
+  <si>
+    <t>GS6111 / Conduct an M985A4 (HEMTT) Hands-on Performance Examination and Critique</t>
+  </si>
+  <si>
+    <t>GH61A1 / Introduction to the M142 Launcher</t>
+  </si>
+  <si>
+    <t>GH61MT / Perform PMCS on an M142 HIMARS Chassis and RSV</t>
+  </si>
+  <si>
+    <t>GH6121 / M142 (HIMARS) Maintenance Hands-On Performance
+Examination</t>
+  </si>
+  <si>
+    <t>GH61DD / Operate an XM1140 Carrier Vehicle during a Fire Mission</t>
+  </si>
+  <si>
+    <t>GH61RL / Perform Driver's Duties during an M142 HIMARS Reload</t>
+  </si>
+  <si>
+    <t>GH6120 / Conduct Driver's Duties Hands-on Performance Examination and Critique on an M142 HIMARS</t>
+  </si>
+  <si>
+    <t>GH61RS / Perform Ammunition Resupply Procedures with an M1084A1P2 RSV with RST</t>
+  </si>
+  <si>
+    <t>GH6111 / Conduct Hands on Performance Examination and Critique on M1084A1P2 RSV Ammunition Resupply Procedures</t>
+  </si>
+  <si>
+    <t>S61SX / Conduct Field Training Exercise</t>
+  </si>
+  <si>
+    <t>GS61IP / Conduct In-Process and Orientation</t>
+  </si>
+  <si>
+    <t>GS61PT / Conduct Physical Readiness Training</t>
+  </si>
+  <si>
+    <t>GS61FR / Conduct Field Training Exercise (FTX) Recovery</t>
+  </si>
+  <si>
+    <t>GS61GR / Conduct End of Course Graduation</t>
+  </si>
+  <si>
+    <t>GS61OP / Conduct Out-Process</t>
+  </si>
+  <si>
+    <t>Verified BY:_________________________________</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -65,11 +153,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -109,8 +192,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,6 +213,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -220,44 +319,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -641,71 +748,318 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="16"/>
-    </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
-    </row>
-    <row r="4" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
+      <c r="A6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="14"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="14"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="14"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="14"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="14"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="14"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="14"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="14"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="14"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="14"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="14"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="14"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="14"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="14"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>